<commit_message>
MVP temp added, multi product friendly
</commit_message>
<xml_diff>
--- a/data/templates/multimarketplace_master_template.xlsx
+++ b/data/templates/multimarketplace_master_template.xlsx
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:JI1"/>
+  <dimension ref="A1:JH1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,8 +501,8 @@
     <col width="14" customWidth="1" min="54" max="54"/>
     <col width="10" customWidth="1" min="55" max="55"/>
     <col width="8" customWidth="1" min="56" max="56"/>
-    <col width="12" customWidth="1" min="57" max="57"/>
-    <col width="15" customWidth="1" min="58" max="58"/>
+    <col width="15" customWidth="1" min="57" max="57"/>
+    <col width="9" customWidth="1" min="58" max="58"/>
     <col width="9" customWidth="1" min="59" max="59"/>
     <col width="9" customWidth="1" min="60" max="60"/>
     <col width="9" customWidth="1" min="61" max="61"/>
@@ -511,8 +511,8 @@
     <col width="9" customWidth="1" min="64" max="64"/>
     <col width="9" customWidth="1" min="65" max="65"/>
     <col width="9" customWidth="1" min="66" max="66"/>
-    <col width="9" customWidth="1" min="67" max="67"/>
-    <col width="10" customWidth="1" min="68" max="68"/>
+    <col width="10" customWidth="1" min="67" max="67"/>
+    <col width="15" customWidth="1" min="68" max="68"/>
     <col width="15" customWidth="1" min="69" max="69"/>
     <col width="15" customWidth="1" min="70" max="70"/>
     <col width="15" customWidth="1" min="71" max="71"/>
@@ -521,7 +521,7 @@
     <col width="15" customWidth="1" min="74" max="74"/>
     <col width="15" customWidth="1" min="75" max="75"/>
     <col width="15" customWidth="1" min="76" max="76"/>
-    <col width="15" customWidth="1" min="77" max="77"/>
+    <col width="19" customWidth="1" min="77" max="77"/>
     <col width="19" customWidth="1" min="78" max="78"/>
     <col width="19" customWidth="1" min="79" max="79"/>
     <col width="19" customWidth="1" min="80" max="80"/>
@@ -529,168 +529,168 @@
     <col width="19" customWidth="1" min="82" max="82"/>
     <col width="19" customWidth="1" min="83" max="83"/>
     <col width="19" customWidth="1" min="84" max="84"/>
-    <col width="19" customWidth="1" min="85" max="85"/>
-    <col width="14" customWidth="1" min="86" max="86"/>
-    <col width="20" customWidth="1" min="87" max="87"/>
-    <col width="12" customWidth="1" min="88" max="88"/>
-    <col width="13" customWidth="1" min="89" max="89"/>
-    <col width="15" customWidth="1" min="90" max="90"/>
-    <col width="41" customWidth="1" min="91" max="91"/>
-    <col width="36" customWidth="1" min="92" max="92"/>
+    <col width="14" customWidth="1" min="85" max="85"/>
+    <col width="20" customWidth="1" min="86" max="86"/>
+    <col width="12" customWidth="1" min="87" max="87"/>
+    <col width="13" customWidth="1" min="88" max="88"/>
+    <col width="15" customWidth="1" min="89" max="89"/>
+    <col width="41" customWidth="1" min="90" max="90"/>
+    <col width="36" customWidth="1" min="91" max="91"/>
+    <col width="24" customWidth="1" min="92" max="92"/>
     <col width="24" customWidth="1" min="93" max="93"/>
-    <col width="24" customWidth="1" min="94" max="94"/>
-    <col width="23" customWidth="1" min="95" max="95"/>
-    <col width="20" customWidth="1" min="96" max="96"/>
-    <col width="19" customWidth="1" min="97" max="97"/>
+    <col width="23" customWidth="1" min="94" max="94"/>
+    <col width="20" customWidth="1" min="95" max="95"/>
+    <col width="19" customWidth="1" min="96" max="96"/>
+    <col width="26" customWidth="1" min="97" max="97"/>
     <col width="26" customWidth="1" min="98" max="98"/>
-    <col width="26" customWidth="1" min="99" max="99"/>
-    <col width="13" customWidth="1" min="100" max="100"/>
-    <col width="20" customWidth="1" min="101" max="101"/>
-    <col width="21" customWidth="1" min="102" max="102"/>
-    <col width="23" customWidth="1" min="103" max="103"/>
+    <col width="13" customWidth="1" min="99" max="99"/>
+    <col width="20" customWidth="1" min="100" max="100"/>
+    <col width="21" customWidth="1" min="101" max="101"/>
+    <col width="23" customWidth="1" min="102" max="102"/>
+    <col width="30" customWidth="1" min="103" max="103"/>
     <col width="30" customWidth="1" min="104" max="104"/>
     <col width="30" customWidth="1" min="105" max="105"/>
-    <col width="30" customWidth="1" min="106" max="106"/>
-    <col width="23" customWidth="1" min="107" max="107"/>
+    <col width="23" customWidth="1" min="106" max="106"/>
+    <col width="19" customWidth="1" min="107" max="107"/>
     <col width="19" customWidth="1" min="108" max="108"/>
-    <col width="19" customWidth="1" min="109" max="109"/>
-    <col width="25" customWidth="1" min="110" max="110"/>
-    <col width="19" customWidth="1" min="111" max="111"/>
-    <col width="12" customWidth="1" min="112" max="112"/>
+    <col width="25" customWidth="1" min="109" max="109"/>
+    <col width="19" customWidth="1" min="110" max="110"/>
+    <col width="12" customWidth="1" min="111" max="111"/>
+    <col width="21" customWidth="1" min="112" max="112"/>
     <col width="21" customWidth="1" min="113" max="113"/>
     <col width="21" customWidth="1" min="114" max="114"/>
-    <col width="21" customWidth="1" min="115" max="115"/>
-    <col width="17" customWidth="1" min="116" max="116"/>
-    <col width="11" customWidth="1" min="117" max="117"/>
-    <col width="27" customWidth="1" min="118" max="118"/>
-    <col width="12" customWidth="1" min="119" max="119"/>
-    <col width="14" customWidth="1" min="120" max="120"/>
-    <col width="21" customWidth="1" min="121" max="121"/>
+    <col width="17" customWidth="1" min="115" max="115"/>
+    <col width="11" customWidth="1" min="116" max="116"/>
+    <col width="27" customWidth="1" min="117" max="117"/>
+    <col width="12" customWidth="1" min="118" max="118"/>
+    <col width="14" customWidth="1" min="119" max="119"/>
+    <col width="21" customWidth="1" min="120" max="120"/>
+    <col width="16" customWidth="1" min="121" max="121"/>
     <col width="16" customWidth="1" min="122" max="122"/>
     <col width="16" customWidth="1" min="123" max="123"/>
-    <col width="16" customWidth="1" min="124" max="124"/>
-    <col width="15" customWidth="1" min="125" max="125"/>
-    <col width="14" customWidth="1" min="126" max="126"/>
-    <col width="22" customWidth="1" min="127" max="127"/>
+    <col width="15" customWidth="1" min="124" max="124"/>
+    <col width="14" customWidth="1" min="125" max="125"/>
+    <col width="22" customWidth="1" min="126" max="126"/>
+    <col width="15" customWidth="1" min="127" max="127"/>
     <col width="15" customWidth="1" min="128" max="128"/>
-    <col width="15" customWidth="1" min="129" max="129"/>
+    <col width="38" customWidth="1" min="129" max="129"/>
     <col width="38" customWidth="1" min="130" max="130"/>
-    <col width="38" customWidth="1" min="131" max="131"/>
-    <col width="8" customWidth="1" min="132" max="132"/>
-    <col width="13" customWidth="1" min="133" max="133"/>
-    <col width="22" customWidth="1" min="134" max="134"/>
-    <col width="10" customWidth="1" min="135" max="135"/>
-    <col width="45" customWidth="1" min="136" max="136"/>
-    <col width="31" customWidth="1" min="137" max="137"/>
-    <col width="14" customWidth="1" min="138" max="138"/>
-    <col width="8" customWidth="1" min="139" max="139"/>
-    <col width="14" customWidth="1" min="140" max="140"/>
+    <col width="8" customWidth="1" min="131" max="131"/>
+    <col width="13" customWidth="1" min="132" max="132"/>
+    <col width="22" customWidth="1" min="133" max="133"/>
+    <col width="10" customWidth="1" min="134" max="134"/>
+    <col width="45" customWidth="1" min="135" max="135"/>
+    <col width="31" customWidth="1" min="136" max="136"/>
+    <col width="14" customWidth="1" min="137" max="137"/>
+    <col width="8" customWidth="1" min="138" max="138"/>
+    <col width="14" customWidth="1" min="139" max="139"/>
+    <col width="33" customWidth="1" min="140" max="140"/>
     <col width="33" customWidth="1" min="141" max="141"/>
     <col width="33" customWidth="1" min="142" max="142"/>
     <col width="33" customWidth="1" min="143" max="143"/>
-    <col width="33" customWidth="1" min="144" max="144"/>
+    <col width="17" customWidth="1" min="144" max="144"/>
     <col width="17" customWidth="1" min="145" max="145"/>
     <col width="17" customWidth="1" min="146" max="146"/>
     <col width="17" customWidth="1" min="147" max="147"/>
     <col width="17" customWidth="1" min="148" max="148"/>
-    <col width="17" customWidth="1" min="149" max="149"/>
-    <col width="21" customWidth="1" min="150" max="150"/>
-    <col width="20" customWidth="1" min="151" max="151"/>
-    <col width="8" customWidth="1" min="152" max="152"/>
-    <col width="22" customWidth="1" min="153" max="153"/>
-    <col width="14" customWidth="1" min="154" max="154"/>
-    <col width="13" customWidth="1" min="155" max="155"/>
-    <col width="8" customWidth="1" min="156" max="156"/>
-    <col width="13" customWidth="1" min="157" max="157"/>
-    <col width="15" customWidth="1" min="158" max="158"/>
-    <col width="7" customWidth="1" min="159" max="159"/>
-    <col width="36" customWidth="1" min="160" max="160"/>
-    <col width="39" customWidth="1" min="161" max="161"/>
-    <col width="20" customWidth="1" min="162" max="162"/>
-    <col width="19" customWidth="1" min="163" max="163"/>
-    <col width="23" customWidth="1" min="164" max="164"/>
+    <col width="21" customWidth="1" min="149" max="149"/>
+    <col width="20" customWidth="1" min="150" max="150"/>
+    <col width="8" customWidth="1" min="151" max="151"/>
+    <col width="22" customWidth="1" min="152" max="152"/>
+    <col width="14" customWidth="1" min="153" max="153"/>
+    <col width="13" customWidth="1" min="154" max="154"/>
+    <col width="8" customWidth="1" min="155" max="155"/>
+    <col width="13" customWidth="1" min="156" max="156"/>
+    <col width="15" customWidth="1" min="157" max="157"/>
+    <col width="7" customWidth="1" min="158" max="158"/>
+    <col width="36" customWidth="1" min="159" max="159"/>
+    <col width="39" customWidth="1" min="160" max="160"/>
+    <col width="20" customWidth="1" min="161" max="161"/>
+    <col width="19" customWidth="1" min="162" max="162"/>
+    <col width="23" customWidth="1" min="163" max="163"/>
+    <col width="26" customWidth="1" min="164" max="164"/>
     <col width="26" customWidth="1" min="165" max="165"/>
-    <col width="26" customWidth="1" min="166" max="166"/>
-    <col width="21" customWidth="1" min="167" max="167"/>
-    <col width="19" customWidth="1" min="168" max="168"/>
-    <col width="32" customWidth="1" min="169" max="169"/>
-    <col width="16" customWidth="1" min="170" max="170"/>
+    <col width="21" customWidth="1" min="166" max="166"/>
+    <col width="19" customWidth="1" min="167" max="167"/>
+    <col width="32" customWidth="1" min="168" max="168"/>
+    <col width="16" customWidth="1" min="169" max="169"/>
+    <col width="14" customWidth="1" min="170" max="170"/>
     <col width="14" customWidth="1" min="171" max="171"/>
     <col width="14" customWidth="1" min="172" max="172"/>
-    <col width="14" customWidth="1" min="173" max="173"/>
-    <col width="10" customWidth="1" min="174" max="174"/>
-    <col width="9" customWidth="1" min="175" max="175"/>
-    <col width="18" customWidth="1" min="176" max="176"/>
-    <col width="19" customWidth="1" min="177" max="177"/>
-    <col width="24" customWidth="1" min="178" max="178"/>
-    <col width="47" customWidth="1" min="179" max="179"/>
-    <col width="23" customWidth="1" min="180" max="180"/>
+    <col width="10" customWidth="1" min="173" max="173"/>
+    <col width="9" customWidth="1" min="174" max="174"/>
+    <col width="18" customWidth="1" min="175" max="175"/>
+    <col width="19" customWidth="1" min="176" max="176"/>
+    <col width="24" customWidth="1" min="177" max="177"/>
+    <col width="47" customWidth="1" min="178" max="178"/>
+    <col width="23" customWidth="1" min="179" max="179"/>
+    <col width="19" customWidth="1" min="180" max="180"/>
     <col width="19" customWidth="1" min="181" max="181"/>
     <col width="19" customWidth="1" min="182" max="182"/>
-    <col width="19" customWidth="1" min="183" max="183"/>
-    <col width="15" customWidth="1" min="184" max="184"/>
-    <col width="24" customWidth="1" min="185" max="185"/>
-    <col width="27" customWidth="1" min="186" max="186"/>
-    <col width="6" customWidth="1" min="187" max="187"/>
-    <col width="19" customWidth="1" min="188" max="188"/>
-    <col width="16" customWidth="1" min="189" max="189"/>
+    <col width="15" customWidth="1" min="183" max="183"/>
+    <col width="24" customWidth="1" min="184" max="184"/>
+    <col width="27" customWidth="1" min="185" max="185"/>
+    <col width="6" customWidth="1" min="186" max="186"/>
+    <col width="19" customWidth="1" min="187" max="187"/>
+    <col width="16" customWidth="1" min="188" max="188"/>
+    <col width="21" customWidth="1" min="189" max="189"/>
     <col width="21" customWidth="1" min="190" max="190"/>
     <col width="21" customWidth="1" min="191" max="191"/>
-    <col width="21" customWidth="1" min="192" max="192"/>
-    <col width="11" customWidth="1" min="193" max="193"/>
-    <col width="18" customWidth="1" min="194" max="194"/>
-    <col width="22" customWidth="1" min="195" max="195"/>
-    <col width="15" customWidth="1" min="196" max="196"/>
-    <col width="11" customWidth="1" min="197" max="197"/>
-    <col width="35" customWidth="1" min="198" max="198"/>
-    <col width="22" customWidth="1" min="199" max="199"/>
-    <col width="25" customWidth="1" min="200" max="200"/>
-    <col width="21" customWidth="1" min="201" max="201"/>
-    <col width="19" customWidth="1" min="202" max="202"/>
-    <col width="32" customWidth="1" min="203" max="203"/>
-    <col width="14" customWidth="1" min="204" max="204"/>
-    <col width="18" customWidth="1" min="205" max="205"/>
-    <col width="15" customWidth="1" min="206" max="206"/>
-    <col width="20" customWidth="1" min="207" max="207"/>
-    <col width="28" customWidth="1" min="208" max="208"/>
-    <col width="9" customWidth="1" min="209" max="209"/>
-    <col width="7" customWidth="1" min="210" max="210"/>
-    <col width="10" customWidth="1" min="211" max="211"/>
-    <col width="19" customWidth="1" min="212" max="212"/>
+    <col width="11" customWidth="1" min="192" max="192"/>
+    <col width="18" customWidth="1" min="193" max="193"/>
+    <col width="22" customWidth="1" min="194" max="194"/>
+    <col width="15" customWidth="1" min="195" max="195"/>
+    <col width="11" customWidth="1" min="196" max="196"/>
+    <col width="35" customWidth="1" min="197" max="197"/>
+    <col width="22" customWidth="1" min="198" max="198"/>
+    <col width="25" customWidth="1" min="199" max="199"/>
+    <col width="21" customWidth="1" min="200" max="200"/>
+    <col width="19" customWidth="1" min="201" max="201"/>
+    <col width="32" customWidth="1" min="202" max="202"/>
+    <col width="14" customWidth="1" min="203" max="203"/>
+    <col width="18" customWidth="1" min="204" max="204"/>
+    <col width="15" customWidth="1" min="205" max="205"/>
+    <col width="20" customWidth="1" min="206" max="206"/>
+    <col width="28" customWidth="1" min="207" max="207"/>
+    <col width="9" customWidth="1" min="208" max="208"/>
+    <col width="7" customWidth="1" min="209" max="209"/>
+    <col width="10" customWidth="1" min="210" max="210"/>
+    <col width="19" customWidth="1" min="211" max="211"/>
+    <col width="50" customWidth="1" min="212" max="212"/>
     <col width="50" customWidth="1" min="213" max="213"/>
     <col width="50" customWidth="1" min="214" max="214"/>
     <col width="50" customWidth="1" min="215" max="215"/>
     <col width="50" customWidth="1" min="216" max="216"/>
-    <col width="50" customWidth="1" min="217" max="217"/>
-    <col width="15" customWidth="1" min="218" max="218"/>
-    <col width="14" customWidth="1" min="219" max="219"/>
+    <col width="15" customWidth="1" min="217" max="217"/>
+    <col width="14" customWidth="1" min="218" max="218"/>
+    <col width="41" customWidth="1" min="219" max="219"/>
     <col width="41" customWidth="1" min="220" max="220"/>
     <col width="41" customWidth="1" min="221" max="221"/>
     <col width="41" customWidth="1" min="222" max="222"/>
-    <col width="41" customWidth="1" min="223" max="223"/>
-    <col width="19" customWidth="1" min="224" max="224"/>
-    <col width="14" customWidth="1" min="225" max="225"/>
-    <col width="19" customWidth="1" min="226" max="226"/>
+    <col width="19" customWidth="1" min="223" max="223"/>
+    <col width="14" customWidth="1" min="224" max="224"/>
+    <col width="19" customWidth="1" min="225" max="225"/>
+    <col width="10" customWidth="1" min="226" max="226"/>
     <col width="10" customWidth="1" min="227" max="227"/>
-    <col width="10" customWidth="1" min="228" max="228"/>
-    <col width="16" customWidth="1" min="229" max="229"/>
-    <col width="18" customWidth="1" min="230" max="230"/>
-    <col width="16" customWidth="1" min="231" max="231"/>
-    <col width="28" customWidth="1" min="232" max="232"/>
-    <col width="19" customWidth="1" min="233" max="233"/>
-    <col width="15" customWidth="1" min="234" max="234"/>
-    <col width="16" customWidth="1" min="235" max="235"/>
-    <col width="13" customWidth="1" min="236" max="236"/>
-    <col width="32" customWidth="1" min="237" max="237"/>
-    <col width="16" customWidth="1" min="238" max="238"/>
-    <col width="18" customWidth="1" min="239" max="239"/>
-    <col width="17" customWidth="1" min="240" max="240"/>
-    <col width="23" customWidth="1" min="241" max="241"/>
-    <col width="17" customWidth="1" min="242" max="242"/>
-    <col width="35" customWidth="1" min="243" max="243"/>
-    <col width="8" customWidth="1" min="244" max="244"/>
-    <col width="7" customWidth="1" min="245" max="245"/>
-    <col width="33" customWidth="1" min="246" max="246"/>
+    <col width="16" customWidth="1" min="228" max="228"/>
+    <col width="18" customWidth="1" min="229" max="229"/>
+    <col width="16" customWidth="1" min="230" max="230"/>
+    <col width="28" customWidth="1" min="231" max="231"/>
+    <col width="19" customWidth="1" min="232" max="232"/>
+    <col width="15" customWidth="1" min="233" max="233"/>
+    <col width="16" customWidth="1" min="234" max="234"/>
+    <col width="13" customWidth="1" min="235" max="235"/>
+    <col width="32" customWidth="1" min="236" max="236"/>
+    <col width="16" customWidth="1" min="237" max="237"/>
+    <col width="18" customWidth="1" min="238" max="238"/>
+    <col width="17" customWidth="1" min="239" max="239"/>
+    <col width="23" customWidth="1" min="240" max="240"/>
+    <col width="17" customWidth="1" min="241" max="241"/>
+    <col width="35" customWidth="1" min="242" max="242"/>
+    <col width="8" customWidth="1" min="243" max="243"/>
+    <col width="7" customWidth="1" min="244" max="244"/>
+    <col width="33" customWidth="1" min="245" max="245"/>
+    <col width="36" customWidth="1" min="246" max="246"/>
     <col width="36" customWidth="1" min="247" max="247"/>
     <col width="36" customWidth="1" min="248" max="248"/>
     <col width="36" customWidth="1" min="249" max="249"/>
@@ -700,20 +700,19 @@
     <col width="36" customWidth="1" min="253" max="253"/>
     <col width="36" customWidth="1" min="254" max="254"/>
     <col width="36" customWidth="1" min="255" max="255"/>
-    <col width="36" customWidth="1" min="256" max="256"/>
-    <col width="50" customWidth="1" min="257" max="257"/>
-    <col width="15" customWidth="1" min="258" max="258"/>
-    <col width="39" customWidth="1" min="259" max="259"/>
-    <col width="15" customWidth="1" min="260" max="260"/>
-    <col width="23" customWidth="1" min="261" max="261"/>
-    <col width="21" customWidth="1" min="262" max="262"/>
-    <col width="19" customWidth="1" min="263" max="263"/>
+    <col width="50" customWidth="1" min="256" max="256"/>
+    <col width="15" customWidth="1" min="257" max="257"/>
+    <col width="39" customWidth="1" min="258" max="258"/>
+    <col width="15" customWidth="1" min="259" max="259"/>
+    <col width="23" customWidth="1" min="260" max="260"/>
+    <col width="21" customWidth="1" min="261" max="261"/>
+    <col width="19" customWidth="1" min="262" max="262"/>
+    <col width="23" customWidth="1" min="263" max="263"/>
     <col width="23" customWidth="1" min="264" max="264"/>
     <col width="23" customWidth="1" min="265" max="265"/>
     <col width="23" customWidth="1" min="266" max="266"/>
-    <col width="23" customWidth="1" min="267" max="267"/>
-    <col width="32" customWidth="1" min="268" max="268"/>
-    <col width="33" customWidth="1" min="269" max="269"/>
+    <col width="32" customWidth="1" min="267" max="267"/>
+    <col width="33" customWidth="1" min="268" max="268"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -999,1072 +998,1067 @@
       </c>
       <c r="BE1" s="3" t="inlineStr">
         <is>
-          <t>Main Color</t>
-        </is>
-      </c>
-      <c r="BF1" s="3" t="inlineStr">
-        <is>
           <t>Main Material</t>
         </is>
       </c>
-      <c r="BG1" s="1" t="inlineStr">
+      <c r="BF1" s="1" t="inlineStr">
         <is>
           <t>Image 1</t>
         </is>
       </c>
+      <c r="BG1" s="2" t="inlineStr">
+        <is>
+          <t>Image 2</t>
+        </is>
+      </c>
       <c r="BH1" s="2" t="inlineStr">
         <is>
-          <t>Image 2</t>
+          <t>Image 3</t>
         </is>
       </c>
       <c r="BI1" s="2" t="inlineStr">
         <is>
-          <t>Image 3</t>
+          <t>Image 4</t>
         </is>
       </c>
       <c r="BJ1" s="2" t="inlineStr">
         <is>
-          <t>Image 4</t>
+          <t>Image 5</t>
         </is>
       </c>
       <c r="BK1" s="2" t="inlineStr">
         <is>
-          <t>Image 5</t>
+          <t>Image 6</t>
         </is>
       </c>
       <c r="BL1" s="2" t="inlineStr">
         <is>
-          <t>Image 6</t>
+          <t>Image 7</t>
         </is>
       </c>
       <c r="BM1" s="2" t="inlineStr">
         <is>
-          <t>Image 7</t>
+          <t>Image 8</t>
         </is>
       </c>
       <c r="BN1" s="2" t="inlineStr">
         <is>
-          <t>Image 8</t>
+          <t>Image 9</t>
         </is>
       </c>
       <c r="BO1" s="2" t="inlineStr">
         <is>
-          <t>Image 9</t>
+          <t>Image 10</t>
         </is>
       </c>
       <c r="BP1" s="2" t="inlineStr">
         <is>
-          <t>Image 10</t>
+          <t>Image Large 1</t>
         </is>
       </c>
       <c r="BQ1" s="2" t="inlineStr">
         <is>
-          <t>Image Large 1</t>
+          <t>Image Large 2</t>
         </is>
       </c>
       <c r="BR1" s="2" t="inlineStr">
         <is>
-          <t>Image Large 2</t>
+          <t>Image Large 3</t>
         </is>
       </c>
       <c r="BS1" s="2" t="inlineStr">
         <is>
-          <t>Image Large 3</t>
+          <t>Image Large 4</t>
         </is>
       </c>
       <c r="BT1" s="2" t="inlineStr">
         <is>
-          <t>Image Large 4</t>
+          <t>Image Large 5</t>
         </is>
       </c>
       <c r="BU1" s="2" t="inlineStr">
         <is>
-          <t>Image Large 5</t>
+          <t>Image Large 6</t>
         </is>
       </c>
       <c r="BV1" s="2" t="inlineStr">
         <is>
-          <t>Image Large 6</t>
+          <t>Image Large 7</t>
         </is>
       </c>
       <c r="BW1" s="2" t="inlineStr">
         <is>
-          <t>Image Large 7</t>
+          <t>Image Large 8</t>
         </is>
       </c>
       <c r="BX1" s="2" t="inlineStr">
         <is>
-          <t>Image Large 8</t>
+          <t>Image Large 9</t>
         </is>
       </c>
       <c r="BY1" s="2" t="inlineStr">
         <is>
-          <t>Image Large 9</t>
+          <t>Secondary Image 1</t>
         </is>
       </c>
       <c r="BZ1" s="2" t="inlineStr">
         <is>
-          <t>Secondary Image 1</t>
+          <t>Secondary Image 2</t>
         </is>
       </c>
       <c r="CA1" s="2" t="inlineStr">
         <is>
-          <t>Secondary Image 2</t>
+          <t>Secondary Image 3</t>
         </is>
       </c>
       <c r="CB1" s="2" t="inlineStr">
         <is>
-          <t>Secondary Image 3</t>
+          <t>Secondary Image 4</t>
         </is>
       </c>
       <c r="CC1" s="2" t="inlineStr">
         <is>
-          <t>Secondary Image 4</t>
+          <t>Secondary Image 5</t>
         </is>
       </c>
       <c r="CD1" s="2" t="inlineStr">
         <is>
-          <t>Secondary Image 5</t>
+          <t>Secondary Image 6</t>
         </is>
       </c>
       <c r="CE1" s="2" t="inlineStr">
         <is>
-          <t>Secondary Image 6</t>
+          <t>Secondary Image 7</t>
         </is>
       </c>
       <c r="CF1" s="2" t="inlineStr">
         <is>
-          <t>Secondary Image 7</t>
+          <t>Secondary Image 8</t>
         </is>
       </c>
       <c r="CG1" s="2" t="inlineStr">
         <is>
-          <t>Secondary Image 8</t>
+          <t>Main Image 1</t>
         </is>
       </c>
       <c r="CH1" s="2" t="inlineStr">
         <is>
-          <t>Main Image 1</t>
-        </is>
-      </c>
-      <c r="CI1" s="2" t="inlineStr">
-        <is>
           <t>Back of Pack Image</t>
         </is>
       </c>
+      <c r="CI1" s="3" t="inlineStr">
+        <is>
+          <t>Can be cut</t>
+        </is>
+      </c>
       <c r="CJ1" s="3" t="inlineStr">
         <is>
-          <t>Can be cut</t>
+          <t>Cut to size</t>
         </is>
       </c>
       <c r="CK1" s="3" t="inlineStr">
         <is>
-          <t>Cut to size</t>
+          <t>Contains wood</t>
         </is>
       </c>
       <c r="CL1" s="3" t="inlineStr">
         <is>
-          <t>Contains wood</t>
+          <t>Compatible with damp rooms or bathrooms</t>
         </is>
       </c>
       <c r="CM1" s="3" t="inlineStr">
         <is>
-          <t>Compatible with damp rooms or bathrooms</t>
+          <t>Suitable for damp spaces indicator</t>
         </is>
       </c>
       <c r="CN1" s="3" t="inlineStr">
         <is>
-          <t>Suitable for damp spaces indicator</t>
+          <t>Usable in humid spaces</t>
         </is>
       </c>
       <c r="CO1" s="3" t="inlineStr">
         <is>
-          <t>Usable in humid spaces</t>
+          <t>Resistant to limescale</t>
         </is>
       </c>
       <c r="CP1" s="3" t="inlineStr">
         <is>
-          <t>Resistant to limescale</t>
+          <t>Resistant to moisture</t>
         </is>
       </c>
       <c r="CQ1" s="3" t="inlineStr">
         <is>
-          <t>Resistant to moisture</t>
+          <t>Resistant to mould</t>
         </is>
       </c>
       <c r="CR1" s="3" t="inlineStr">
         <is>
-          <t>Resistant to mould</t>
+          <t>Resistant to rust</t>
         </is>
       </c>
       <c r="CS1" s="3" t="inlineStr">
         <is>
-          <t>Resistant to rust</t>
+          <t>Resistant to ultraviolet</t>
         </is>
       </c>
       <c r="CT1" s="3" t="inlineStr">
         <is>
-          <t>Resistant to ultraviolet</t>
+          <t>Fire-retardant indicator</t>
         </is>
       </c>
       <c r="CU1" s="3" t="inlineStr">
         <is>
-          <t>Fire-retardant indicator</t>
+          <t>UKCA marked</t>
         </is>
       </c>
       <c r="CV1" s="3" t="inlineStr">
         <is>
-          <t>UKCA marked</t>
+          <t>FSC Mark indicator</t>
         </is>
       </c>
       <c r="CW1" s="3" t="inlineStr">
         <is>
-          <t>FSC Mark indicator</t>
+          <t>PEFC mark indicator</t>
         </is>
       </c>
       <c r="CX1" s="3" t="inlineStr">
         <is>
-          <t>PEFC mark indicator</t>
+          <t>Accessories available</t>
         </is>
       </c>
       <c r="CY1" s="3" t="inlineStr">
         <is>
-          <t>Accessories available</t>
+          <t>Accessories included (fr_BE)</t>
         </is>
       </c>
       <c r="CZ1" s="3" t="inlineStr">
         <is>
-          <t>Accessories included (fr_BE)</t>
+          <t>Accessories included (nl_BE)</t>
         </is>
       </c>
       <c r="DA1" s="3" t="inlineStr">
         <is>
-          <t>Accessories included (nl_BE)</t>
+          <t>Accessories included (nl_NL)</t>
         </is>
       </c>
       <c r="DB1" s="3" t="inlineStr">
         <is>
-          <t>Accessories included (nl_NL)</t>
+          <t>Acquisition CE marked</t>
         </is>
       </c>
       <c r="DC1" s="3" t="inlineStr">
         <is>
-          <t>Acquisition CE marked</t>
+          <t>Acquisition brand</t>
         </is>
       </c>
       <c r="DD1" s="3" t="inlineStr">
         <is>
-          <t>Acquisition brand</t>
+          <t>Adhesive required</t>
         </is>
       </c>
       <c r="DE1" s="3" t="inlineStr">
         <is>
-          <t>Adhesive required</t>
+          <t>Advantage and benefit 2</t>
         </is>
       </c>
       <c r="DF1" s="3" t="inlineStr">
         <is>
-          <t>Advantage and benefit 2</t>
+          <t>Amount of Content</t>
         </is>
       </c>
       <c r="DG1" s="3" t="inlineStr">
         <is>
-          <t>Amount of Content</t>
+          <t>Appearance</t>
         </is>
       </c>
       <c r="DH1" s="3" t="inlineStr">
         <is>
-          <t>Appearance</t>
+          <t>Application (fr_BE)</t>
         </is>
       </c>
       <c r="DI1" s="3" t="inlineStr">
         <is>
-          <t>Application (fr_BE)</t>
+          <t>Application (nl_BE)</t>
         </is>
       </c>
       <c r="DJ1" s="3" t="inlineStr">
         <is>
-          <t>Application (nl_BE)</t>
+          <t>Application (nl_NL)</t>
         </is>
       </c>
       <c r="DK1" s="3" t="inlineStr">
         <is>
-          <t>Application (nl_NL)</t>
+          <t>Batten material</t>
         </is>
       </c>
       <c r="DL1" s="3" t="inlineStr">
         <is>
-          <t>Batten material</t>
+          <t>Body Copy</t>
         </is>
       </c>
       <c r="DM1" s="3" t="inlineStr">
         <is>
-          <t>Body Copy</t>
-        </is>
-      </c>
-      <c r="DN1" s="3" t="inlineStr">
-        <is>
           <t>Box capacity (in m²) (m²)</t>
         </is>
       </c>
-      <c r="DO1" s="2" t="inlineStr">
+      <c r="DN1" s="2" t="inlineStr">
         <is>
           <t>Brand Name</t>
         </is>
       </c>
+      <c r="DO1" s="3" t="inlineStr">
+        <is>
+          <t>Click system</t>
+        </is>
+      </c>
       <c r="DP1" s="3" t="inlineStr">
         <is>
-          <t>Click system</t>
+          <t>Color of the batten</t>
         </is>
       </c>
       <c r="DQ1" s="3" t="inlineStr">
         <is>
-          <t>Color of the batten</t>
+          <t>Colour (fr_BE)</t>
         </is>
       </c>
       <c r="DR1" s="3" t="inlineStr">
         <is>
-          <t>Colour (fr_BE)</t>
+          <t>Colour (nl_BE)</t>
         </is>
       </c>
       <c r="DS1" s="3" t="inlineStr">
         <is>
-          <t>Colour (nl_BE)</t>
+          <t>Colour (nl_NL)</t>
         </is>
       </c>
       <c r="DT1" s="3" t="inlineStr">
         <is>
-          <t>Colour (nl_NL)</t>
+          <t>Colour family</t>
         </is>
       </c>
       <c r="DU1" s="3" t="inlineStr">
         <is>
-          <t>Colour family</t>
+          <t>Colour group</t>
         </is>
       </c>
       <c r="DV1" s="3" t="inlineStr">
         <is>
-          <t>Colour group</t>
+          <t>Commercial reference</t>
         </is>
       </c>
       <c r="DW1" s="3" t="inlineStr">
         <is>
-          <t>Commercial reference</t>
+          <t>Consumer unit</t>
         </is>
       </c>
       <c r="DX1" s="3" t="inlineStr">
         <is>
-          <t>Consumer unit</t>
+          <t>Coverage (m²)</t>
         </is>
       </c>
       <c r="DY1" s="3" t="inlineStr">
         <is>
-          <t>Coverage (m²)</t>
+          <t>Declaration of Performance Datasheet</t>
         </is>
       </c>
       <c r="DZ1" s="3" t="inlineStr">
         <is>
-          <t>Declaration of Performance Datasheet</t>
+          <t>Depth (without packaging) in cm (cm)</t>
         </is>
       </c>
       <c r="EA1" s="3" t="inlineStr">
         <is>
-          <t>Depth (without packaging) in cm (cm)</t>
+          <t>Design</t>
         </is>
       </c>
       <c r="EB1" s="3" t="inlineStr">
         <is>
-          <t>Design</t>
+          <t>Destination</t>
         </is>
       </c>
       <c r="EC1" s="3" t="inlineStr">
         <is>
-          <t>Destination</t>
+          <t>Detergent Data Sheet</t>
         </is>
       </c>
       <c r="ED1" s="3" t="inlineStr">
         <is>
-          <t>Detergent Data Sheet</t>
+          <t>Document</t>
         </is>
       </c>
       <c r="EE1" s="3" t="inlineStr">
         <is>
-          <t>Document</t>
+          <t>Duration of warranty period (in years) (yr)</t>
         </is>
       </c>
       <c r="EF1" s="3" t="inlineStr">
         <is>
-          <t>Duration of warranty period (in years) (yr)</t>
+          <t>EU Warning_Safety Information</t>
         </is>
       </c>
       <c r="EG1" s="3" t="inlineStr">
         <is>
-          <t>EU Warning_Safety Information</t>
+          <t>Edge profile</t>
         </is>
       </c>
       <c r="EH1" s="3" t="inlineStr">
         <is>
-          <t>Edge profile</t>
+          <t>Effect</t>
         </is>
       </c>
       <c r="EI1" s="3" t="inlineStr">
         <is>
-          <t>Effect</t>
+          <t>Energy Label</t>
         </is>
       </c>
       <c r="EJ1" s="3" t="inlineStr">
         <is>
-          <t>Energy Label</t>
+          <t>Energy Related product label ES</t>
         </is>
       </c>
       <c r="EK1" s="3" t="inlineStr">
         <is>
-          <t>Energy Related product label ES</t>
+          <t>Energy Related product label FR</t>
         </is>
       </c>
       <c r="EL1" s="3" t="inlineStr">
         <is>
-          <t>Energy Related product label FR</t>
+          <t>Energy Related product label IT</t>
         </is>
       </c>
       <c r="EM1" s="3" t="inlineStr">
         <is>
-          <t>Energy Related product label IT</t>
+          <t>Energy Related product label PT</t>
         </is>
       </c>
       <c r="EN1" s="3" t="inlineStr">
         <is>
-          <t>Energy Related product label PT</t>
+          <t>FSC code part 1</t>
         </is>
       </c>
       <c r="EO1" s="3" t="inlineStr">
         <is>
-          <t>FSC code part 1</t>
+          <t>FSC code part 2</t>
         </is>
       </c>
       <c r="EP1" s="3" t="inlineStr">
         <is>
-          <t>FSC code part 2</t>
+          <t>FSC code part 3</t>
         </is>
       </c>
       <c r="EQ1" s="3" t="inlineStr">
         <is>
-          <t>FSC code part 3</t>
+          <t>FSC code part 4</t>
         </is>
       </c>
       <c r="ER1" s="3" t="inlineStr">
         <is>
-          <t>FSC code part 4</t>
+          <t>FSC composition</t>
         </is>
       </c>
       <c r="ES1" s="3" t="inlineStr">
         <is>
-          <t>FSC composition</t>
+          <t>FSC expiration date</t>
         </is>
       </c>
       <c r="ET1" s="3" t="inlineStr">
         <is>
-          <t>FSC expiration date</t>
+          <t>Facet product type</t>
         </is>
       </c>
       <c r="EU1" s="3" t="inlineStr">
         <is>
-          <t>Facet product type</t>
+          <t>Finish</t>
         </is>
       </c>
       <c r="EV1" s="3" t="inlineStr">
         <is>
-          <t>Finish</t>
+          <t>Finishing of product</t>
         </is>
       </c>
       <c r="EW1" s="3" t="inlineStr">
         <is>
-          <t>Finishing of product</t>
+          <t>Fitting type</t>
         </is>
       </c>
       <c r="EX1" s="3" t="inlineStr">
         <is>
-          <t>Fitting type</t>
+          <t>Fixing type</t>
         </is>
       </c>
       <c r="EY1" s="3" t="inlineStr">
         <is>
-          <t>Fixing type</t>
+          <t>Format</t>
         </is>
       </c>
       <c r="EZ1" s="3" t="inlineStr">
         <is>
-          <t>Format</t>
+          <t>GPSR Exempt</t>
         </is>
       </c>
       <c r="FA1" s="3" t="inlineStr">
         <is>
-          <t>GPSR Exempt</t>
+          <t>Gallery Video</t>
         </is>
       </c>
       <c r="FB1" s="3" t="inlineStr">
         <is>
-          <t>Gallery Video</t>
+          <t>Genus</t>
         </is>
       </c>
       <c r="FC1" s="3" t="inlineStr">
         <is>
-          <t>Genus</t>
+          <t>Guarantee exclusion specifications</t>
         </is>
       </c>
       <c r="FD1" s="3" t="inlineStr">
         <is>
-          <t>Guarantee exclusion specifications</t>
+          <t>Height (without packaging) in cm (cm)</t>
         </is>
       </c>
       <c r="FE1" s="3" t="inlineStr">
         <is>
-          <t>Height (without packaging) in cm (cm)</t>
+          <t>Impregnation class</t>
         </is>
       </c>
       <c r="FF1" s="3" t="inlineStr">
         <is>
-          <t>Impregnation class</t>
+          <t>Installation type</t>
         </is>
       </c>
       <c r="FG1" s="3" t="inlineStr">
         <is>
-          <t>Installation type</t>
+          <t>Instructions for care</t>
         </is>
       </c>
       <c r="FH1" s="3" t="inlineStr">
         <is>
-          <t>Instructions for care</t>
+          <t>Instructions for fitting</t>
         </is>
       </c>
       <c r="FI1" s="3" t="inlineStr">
         <is>
-          <t>Instructions for fitting</t>
+          <t>Instructions for storage</t>
         </is>
       </c>
       <c r="FJ1" s="3" t="inlineStr">
         <is>
-          <t>Instructions for storage</t>
+          <t>Insulation material</t>
         </is>
       </c>
       <c r="FK1" s="3" t="inlineStr">
         <is>
-          <t>Insulation material</t>
+          <t>Legal Information</t>
         </is>
       </c>
       <c r="FL1" s="3" t="inlineStr">
         <is>
-          <t>Legal Information</t>
+          <t>Legal Information from Vendors</t>
         </is>
       </c>
       <c r="FM1" s="3" t="inlineStr">
         <is>
-          <t>Legal Information from Vendors</t>
+          <t>Length (in cm)</t>
         </is>
       </c>
       <c r="FN1" s="3" t="inlineStr">
         <is>
-          <t>Length (in cm)</t>
+          <t>Line (fr_BE)</t>
         </is>
       </c>
       <c r="FO1" s="3" t="inlineStr">
         <is>
-          <t>Line (fr_BE)</t>
+          <t>Line (nl_BE)</t>
         </is>
       </c>
       <c r="FP1" s="3" t="inlineStr">
         <is>
-          <t>Line (nl_BE)</t>
+          <t>Line (nl_NL)</t>
         </is>
       </c>
       <c r="FQ1" s="3" t="inlineStr">
         <is>
-          <t>Line (nl_NL)</t>
+          <t>Location</t>
         </is>
       </c>
       <c r="FR1" s="3" t="inlineStr">
         <is>
-          <t>Location</t>
+          <t>Made in</t>
         </is>
       </c>
       <c r="FS1" s="3" t="inlineStr">
         <is>
-          <t>Made in</t>
-        </is>
-      </c>
-      <c r="FT1" s="3" t="inlineStr">
-        <is>
           <t>Made in Portugal</t>
         </is>
       </c>
-      <c r="FU1" s="2" t="inlineStr">
+      <c r="FT1" s="2" t="inlineStr">
         <is>
           <t>Manufacturer Name</t>
         </is>
       </c>
+      <c r="FU1" s="3" t="inlineStr">
+        <is>
+          <t>Manufacturer guarantee</t>
+        </is>
+      </c>
       <c r="FV1" s="3" t="inlineStr">
         <is>
-          <t>Manufacturer guarantee</t>
+          <t>Manufacturer's commercial warranty (in years)</t>
         </is>
       </c>
       <c r="FW1" s="3" t="inlineStr">
         <is>
-          <t>Manufacturer's commercial warranty (in years)</t>
+          <t>Manufacturing country</t>
         </is>
       </c>
       <c r="FX1" s="3" t="inlineStr">
         <is>
-          <t>Manufacturing country</t>
+          <t>Material property</t>
         </is>
       </c>
       <c r="FY1" s="3" t="inlineStr">
         <is>
-          <t>Material property</t>
+          <t>Material specific</t>
         </is>
       </c>
       <c r="FZ1" s="3" t="inlineStr">
         <is>
-          <t>Material specific</t>
+          <t>Model name/number</t>
         </is>
       </c>
       <c r="GA1" s="3" t="inlineStr">
         <is>
-          <t>Model name/number</t>
+          <t>Mounting type</t>
         </is>
       </c>
       <c r="GB1" s="3" t="inlineStr">
         <is>
-          <t>Mounting type</t>
+          <t>Mounting/fixing method</t>
         </is>
       </c>
       <c r="GC1" s="3" t="inlineStr">
         <is>
-          <t>Mounting/fixing method</t>
+          <t>MultiSKU Product Group ID</t>
         </is>
       </c>
       <c r="GD1" s="3" t="inlineStr">
         <is>
-          <t>MultiSKU Product Group ID</t>
+          <t>Name</t>
         </is>
       </c>
       <c r="GE1" s="3" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>Name of the serie</t>
         </is>
       </c>
       <c r="GF1" s="3" t="inlineStr">
         <is>
-          <t>Name of the serie</t>
+          <t>Origin of wood</t>
         </is>
       </c>
       <c r="GG1" s="3" t="inlineStr">
         <is>
-          <t>Origin of wood</t>
+          <t>Other value (fr_BE)</t>
         </is>
       </c>
       <c r="GH1" s="3" t="inlineStr">
         <is>
-          <t>Other value (fr_BE)</t>
+          <t>Other value (nl_BE)</t>
         </is>
       </c>
       <c r="GI1" s="3" t="inlineStr">
         <is>
-          <t>Other value (nl_BE)</t>
+          <t>Other value (nl_NL)</t>
         </is>
       </c>
       <c r="GJ1" s="3" t="inlineStr">
         <is>
-          <t>Other value (nl_NL)</t>
+          <t>PEFC code</t>
         </is>
       </c>
       <c r="GK1" s="3" t="inlineStr">
         <is>
-          <t>PEFC code</t>
+          <t>PEFC composition</t>
         </is>
       </c>
       <c r="GL1" s="3" t="inlineStr">
         <is>
-          <t>PEFC composition</t>
+          <t>PEFC expiration date</t>
         </is>
       </c>
       <c r="GM1" s="3" t="inlineStr">
         <is>
-          <t>PEFC expiration date</t>
+          <t>Pack quantity</t>
         </is>
       </c>
       <c r="GN1" s="3" t="inlineStr">
         <is>
-          <t>Pack quantity</t>
+          <t>Pack type</t>
         </is>
       </c>
       <c r="GO1" s="3" t="inlineStr">
         <is>
-          <t>Pack type</t>
+          <t>Packaged product : weight (in kg)</t>
         </is>
       </c>
       <c r="GP1" s="3" t="inlineStr">
         <is>
-          <t>Packaged product : weight (in kg)</t>
+          <t>Panel height (in cm)</t>
         </is>
       </c>
       <c r="GQ1" s="3" t="inlineStr">
         <is>
-          <t>Panel height (in cm)</t>
+          <t>Panel thickness (in mm)</t>
         </is>
       </c>
       <c r="GR1" s="3" t="inlineStr">
         <is>
-          <t>Panel thickness (in mm)</t>
+          <t>Panel width (in cm)</t>
         </is>
       </c>
       <c r="GS1" s="3" t="inlineStr">
         <is>
-          <t>Panel width (in cm)</t>
+          <t>Parent Product ID</t>
         </is>
       </c>
       <c r="GT1" s="3" t="inlineStr">
         <is>
-          <t>Parent Product ID</t>
+          <t>Performance declaration EN B2B</t>
         </is>
       </c>
       <c r="GU1" s="3" t="inlineStr">
         <is>
-          <t>Performance declaration EN B2B</t>
+          <t>Place of use</t>
         </is>
       </c>
       <c r="GV1" s="3" t="inlineStr">
         <is>
-          <t>Place of use</t>
+          <t>Product Category</t>
         </is>
       </c>
       <c r="GW1" s="3" t="inlineStr">
         <is>
-          <t>Product Category</t>
+          <t>Product Guide</t>
         </is>
       </c>
       <c r="GX1" s="3" t="inlineStr">
         <is>
-          <t>Product Guide</t>
+          <t>Product Identifier</t>
         </is>
       </c>
       <c r="GY1" s="3" t="inlineStr">
         <is>
-          <t>Product Identifier</t>
+          <t>Product Instruction Manual</t>
         </is>
       </c>
       <c r="GZ1" s="3" t="inlineStr">
         <is>
-          <t>Product Instruction Manual</t>
+          <t>Purpose</t>
         </is>
       </c>
       <c r="HA1" s="3" t="inlineStr">
         <is>
-          <t>Purpose</t>
+          <t>Range</t>
         </is>
       </c>
       <c r="HB1" s="3" t="inlineStr">
         <is>
-          <t>Range</t>
+          <t>Room use</t>
         </is>
       </c>
       <c r="HC1" s="3" t="inlineStr">
         <is>
-          <t>Room use</t>
+          <t>Safety Data Sheet</t>
         </is>
       </c>
       <c r="HD1" s="3" t="inlineStr">
         <is>
-          <t>Safety Data Sheet</t>
+          <t>Safety Information Asset 1 - Digital Assets  01W</t>
         </is>
       </c>
       <c r="HE1" s="3" t="inlineStr">
         <is>
-          <t>Safety Information Asset 1 - Digital Assets  01W</t>
+          <t>Safety Information Asset 2 - Digital Assets  02W</t>
         </is>
       </c>
       <c r="HF1" s="3" t="inlineStr">
         <is>
-          <t>Safety Information Asset 2 - Digital Assets  02W</t>
+          <t>Safety Information Asset 3 - Digital Assets  03W</t>
         </is>
       </c>
       <c r="HG1" s="3" t="inlineStr">
         <is>
-          <t>Safety Information Asset 3 - Digital Assets  03W</t>
+          <t>Safety Information Asset 4 - Digital Assets  04W</t>
         </is>
       </c>
       <c r="HH1" s="3" t="inlineStr">
         <is>
-          <t>Safety Information Asset 4 - Digital Assets  04W</t>
+          <t>Safety Information Asset 5 - Digital Assets  05W</t>
         </is>
       </c>
       <c r="HI1" s="3" t="inlineStr">
         <is>
-          <t>Safety Information Asset 5 - Digital Assets  05W</t>
+          <t>Safety Manual</t>
         </is>
       </c>
       <c r="HJ1" s="3" t="inlineStr">
         <is>
-          <t>Safety Manual</t>
+          <t>Sale content</t>
         </is>
       </c>
       <c r="HK1" s="3" t="inlineStr">
         <is>
-          <t>Sale content</t>
+          <t>Security Data Sheet ES - Packaging rear</t>
         </is>
       </c>
       <c r="HL1" s="3" t="inlineStr">
         <is>
-          <t>Security Data Sheet ES - Packaging rear</t>
+          <t>Security Data Sheet FR - Packaging rear</t>
         </is>
       </c>
       <c r="HM1" s="3" t="inlineStr">
         <is>
-          <t>Security Data Sheet FR - Packaging rear</t>
+          <t>Security Data Sheet IT - Packaging rear</t>
         </is>
       </c>
       <c r="HN1" s="3" t="inlineStr">
         <is>
-          <t>Security Data Sheet IT - Packaging rear</t>
+          <t>Security Data Sheet PT - Packaging rear</t>
         </is>
       </c>
       <c r="HO1" s="3" t="inlineStr">
         <is>
-          <t>Security Data Sheet PT - Packaging rear</t>
+          <t>Seller Product ID</t>
         </is>
       </c>
       <c r="HP1" s="3" t="inlineStr">
         <is>
-          <t>Seller Product ID</t>
+          <t>Selling Copy</t>
         </is>
       </c>
       <c r="HQ1" s="3" t="inlineStr">
         <is>
-          <t>Selling Copy</t>
+          <t>Selling unit type</t>
         </is>
       </c>
       <c r="HR1" s="3" t="inlineStr">
         <is>
-          <t>Selling unit type</t>
+          <t>Shop SKU</t>
         </is>
       </c>
       <c r="HS1" s="3" t="inlineStr">
         <is>
-          <t>Shop SKU</t>
+          <t>Standard</t>
         </is>
       </c>
       <c r="HT1" s="3" t="inlineStr">
         <is>
-          <t>Standard</t>
+          <t>Support colour</t>
         </is>
       </c>
       <c r="HU1" s="3" t="inlineStr">
         <is>
-          <t>Support colour</t>
+          <t>Support material</t>
         </is>
       </c>
       <c r="HV1" s="3" t="inlineStr">
         <is>
-          <t>Support material</t>
+          <t>Surface finish</t>
         </is>
       </c>
       <c r="HW1" s="3" t="inlineStr">
         <is>
-          <t>Surface finish</t>
+          <t>Technical document  FR B2B</t>
         </is>
       </c>
       <c r="HX1" s="3" t="inlineStr">
         <is>
-          <t>Technical document  FR B2B</t>
+          <t>Thickness (in mm)</t>
         </is>
       </c>
       <c r="HY1" s="3" t="inlineStr">
         <is>
-          <t>Thickness (in mm)</t>
+          <t>Timber origin</t>
         </is>
       </c>
       <c r="HZ1" s="3" t="inlineStr">
         <is>
-          <t>Timber origin</t>
+          <t>Timber species</t>
         </is>
       </c>
       <c r="IA1" s="3" t="inlineStr">
         <is>
-          <t>Timber species</t>
+          <t>Timber type</t>
         </is>
       </c>
       <c r="IB1" s="3" t="inlineStr">
         <is>
-          <t>Timber type</t>
+          <t>Tools required for the fitting</t>
         </is>
       </c>
       <c r="IC1" s="3" t="inlineStr">
         <is>
-          <t>Tools required for the fitting</t>
+          <t>Type of effect</t>
         </is>
       </c>
       <c r="ID1" s="3" t="inlineStr">
         <is>
-          <t>Type of effect</t>
+          <t>Type of material</t>
         </is>
       </c>
       <c r="IE1" s="3" t="inlineStr">
         <is>
-          <t>Type of material</t>
+          <t>Type of product</t>
         </is>
       </c>
       <c r="IF1" s="3" t="inlineStr">
         <is>
-          <t>Type of product</t>
+          <t>UOM for sales content</t>
         </is>
       </c>
       <c r="IG1" s="3" t="inlineStr">
         <is>
-          <t>UOM for sales content</t>
+          <t>Unit of content</t>
         </is>
       </c>
       <c r="IH1" s="3" t="inlineStr">
         <is>
-          <t>Unit of content</t>
+          <t>VOC emissions class in indoor air</t>
         </is>
       </c>
       <c r="II1" s="3" t="inlineStr">
         <is>
-          <t>VOC emissions class in indoor air</t>
+          <t>Veneer</t>
         </is>
       </c>
       <c r="IJ1" s="3" t="inlineStr">
         <is>
-          <t>Veneer</t>
+          <t>Video</t>
         </is>
       </c>
       <c r="IK1" s="3" t="inlineStr">
         <is>
-          <t>Video</t>
+          <t>Volatil Organism Compound label</t>
         </is>
       </c>
       <c r="IL1" s="3" t="inlineStr">
         <is>
-          <t>Volatil Organism Compound label</t>
+          <t>Warnings and Safety Information 01</t>
         </is>
       </c>
       <c r="IM1" s="3" t="inlineStr">
         <is>
-          <t>Warnings and Safety Information 01</t>
+          <t>Warnings and Safety Information 02</t>
         </is>
       </c>
       <c r="IN1" s="3" t="inlineStr">
         <is>
-          <t>Warnings and Safety Information 02</t>
+          <t>Warnings and Safety Information 03</t>
         </is>
       </c>
       <c r="IO1" s="3" t="inlineStr">
         <is>
-          <t>Warnings and Safety Information 03</t>
+          <t>Warnings and Safety Information 04</t>
         </is>
       </c>
       <c r="IP1" s="3" t="inlineStr">
         <is>
-          <t>Warnings and Safety Information 04</t>
+          <t>Warnings and Safety Information 05</t>
         </is>
       </c>
       <c r="IQ1" s="3" t="inlineStr">
         <is>
-          <t>Warnings and Safety Information 05</t>
+          <t>Warnings and Safety Information 06</t>
         </is>
       </c>
       <c r="IR1" s="3" t="inlineStr">
         <is>
-          <t>Warnings and Safety Information 06</t>
+          <t>Warnings and Safety Information 07</t>
         </is>
       </c>
       <c r="IS1" s="3" t="inlineStr">
         <is>
-          <t>Warnings and Safety Information 07</t>
+          <t>Warnings and Safety Information 08</t>
         </is>
       </c>
       <c r="IT1" s="3" t="inlineStr">
         <is>
-          <t>Warnings and Safety Information 08</t>
+          <t>Warnings and Safety Information 09</t>
         </is>
       </c>
       <c r="IU1" s="3" t="inlineStr">
         <is>
-          <t>Warnings and Safety Information 09</t>
+          <t>Warnings and Safety Information 10</t>
         </is>
       </c>
       <c r="IV1" s="3" t="inlineStr">
         <is>
-          <t>Warnings and Safety Information 10</t>
+          <t>Warranty (in years) (includes the legal conformity warranty)</t>
         </is>
       </c>
       <c r="IW1" s="3" t="inlineStr">
         <is>
-          <t>Warranty (in years) (includes the legal conformity warranty)</t>
+          <t>Washable code</t>
         </is>
       </c>
       <c r="IX1" s="3" t="inlineStr">
         <is>
-          <t>Washable code</t>
+          <t>Width  (without packaging) in cm (cm)</t>
         </is>
       </c>
       <c r="IY1" s="3" t="inlineStr">
         <is>
-          <t>Width  (without packaging) in cm (cm)</t>
+          <t>Width (in cm)</t>
         </is>
       </c>
       <c r="IZ1" s="3" t="inlineStr">
         <is>
-          <t>Width (in cm)</t>
+          <t>Wood durability class</t>
         </is>
       </c>
       <c r="JA1" s="3" t="inlineStr">
         <is>
-          <t>Wood durability class</t>
+          <t>Wood licence number</t>
         </is>
       </c>
       <c r="JB1" s="3" t="inlineStr">
         <is>
-          <t>Wood licence number</t>
+          <t>Wood pretreatment</t>
         </is>
       </c>
       <c r="JC1" s="3" t="inlineStr">
         <is>
-          <t>Wood pretreatment</t>
+          <t>instruction in PDF ES</t>
         </is>
       </c>
       <c r="JD1" s="3" t="inlineStr">
         <is>
-          <t>instruction in PDF ES</t>
+          <t>instruction in PDF FR</t>
         </is>
       </c>
       <c r="JE1" s="3" t="inlineStr">
         <is>
-          <t>instruction in PDF FR</t>
+          <t>instruction in PDF IT</t>
         </is>
       </c>
       <c r="JF1" s="3" t="inlineStr">
         <is>
-          <t>instruction in PDF IT</t>
+          <t>instruction in PDF PT</t>
         </is>
       </c>
       <c r="JG1" s="3" t="inlineStr">
         <is>
-          <t>instruction in PDF PT</t>
+          <t>wood_certificate_fsc_indicator</t>
         </is>
       </c>
       <c r="JH1" s="3" t="inlineStr">
-        <is>
-          <t>wood_certificate_fsc_indicator</t>
-        </is>
-      </c>
-      <c r="JI1" s="3" t="inlineStr">
         <is>
           <t>wood_certificate_pefc_indicator</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="15">
+  <dataValidations count="14">
     <dataValidation sqref="A2:A1000" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Flooring,Furniture,Lighting,Kitchen,Bathroom,Garden,Tools,Paint,Hardware,Decor,Storage,Outdoor,Indoor,Commercial,Residential,Wall Covering,Ceiling,Window,Door,Staircase,Fencing,Decking"</formula1>
     </dataValidation>
@@ -2075,39 +2069,36 @@
       <formula1>"White,Black,Brown,Grey,Beige,Blue,Red,Green,Yellow,Orange,Purple,Pink,Multi,Natural,Oak,Walnut,Mahogany,Pine,Cedar,Maple,Cherry,Teak,Ash,Birch,Elm,Poplar,Spruce,Fir,Larch"</formula1>
     </dataValidation>
     <dataValidation sqref="BE2:BE1000" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>"White,Black,Brown,Grey,Beige,Blue,Red,Green,Yellow,Orange,Purple,Pink,Multi,Natural,Oak,Walnut,Mahogany,Pine,Cedar,Maple,Cherry,Teak,Ash,Birch,Elm,Poplar,Spruce,Fir,Larch"</formula1>
-    </dataValidation>
-    <dataValidation sqref="BF2:BF1000" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Wood,Metal,Plastic,Glass,Ceramic,Fabric,Leather,Synthetic,Natural,Composite,Aluminum,Steel,Iron,Copper,Bronze,Stone,Marble,Granite,Concrete,Bamboo,Cork,Rattan,Wicker,Particle Board,MDF,Plywood,Solid Wood,Engineered Wood"</formula1>
     </dataValidation>
-    <dataValidation sqref="CJ2:CJ1000" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="CI2:CI1000" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation sqref="CL2:CL1000" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="CK2:CK1000" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation sqref="CV2:CV1000" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="CU2:CU1000" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation sqref="DC2:DC1000" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="DB2:DB1000" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation sqref="EB2:EB1000" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="EA2:EA1000" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Traditional,Modern,Contemporary,Rustic,Industrial,Scandinavian,Minimalist,Vintage,Art Deco,Victorian,Mediterranean,Asian,Bohemian,Shabby Chic,Farmhouse"</formula1>
     </dataValidation>
-    <dataValidation sqref="EI2:EI1000" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="EH2:EH1000" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"None,Distressed,Aged,Weathered,Antique,Vintage,Hand-scraped,Wire-brushed,Smooth,Textured,Embossed,Grooved,Chamfered,Beveled,Rounded,Square"</formula1>
     </dataValidation>
-    <dataValidation sqref="EV2:EV1000" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="EU2:EU1000" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Natural,Stained,Painted,Varnished,Oiled,Waxed,Lacquered,Distressed,Aged,Rustic,Modern,Classic,Glossy,Matte,Satin,Semi-gloss,Textured,Smooth"</formula1>
     </dataValidation>
-    <dataValidation sqref="FA2:FA1000" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="EZ2:EZ1000" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation sqref="FT2:FT1000" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="FS2:FS1000" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation sqref="GW2:GW1000" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="GV2:GV1000" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Flooring,Furniture,Lighting,Kitchen,Bathroom,Garden,Tools,Paint,Hardware,Decor,Storage,Outdoor,Indoor,Commercial,Residential,Wall Covering,Ceiling,Window,Door,Staircase,Fencing,Decking"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>